<commit_message>
* create definition of LocalSettingStore for blancoPinia * add definition for .gitignore
</commit_message>
<xml_diff>
--- a/meta/stores/PageTransitDataStore.xlsx
+++ b/meta/stores/PageTransitDataStore.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10520"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11010"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/dapanda/dapanda-front-core/meta/stores/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yhaino/Desktop/dapanda-front-core/meta/stores/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5881AFE4-6439-7047-BF99-3383849EA9A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17869D26-A40A-D742-8020-54E605FB6F43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="VueStore" sheetId="1" r:id="rId1"/>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="63">
   <si>
     <t>パッケージ</t>
   </si>
@@ -636,7 +636,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="45">
+  <borders count="49">
     <border>
       <left/>
       <right/>
@@ -1170,12 +1170,62 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="hair">
+        <color indexed="8"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="hair">
+        <color indexed="8"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="hair">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="114">
+  <cellXfs count="116">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -1336,9 +1386,45 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1360,48 +1446,10 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
@@ -1815,8 +1863,8 @@
   </sheetPr>
   <dimension ref="A1:K98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="F80" sqref="F80"/>
+    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
+      <selection activeCell="I82" sqref="I82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -1890,10 +1938,10 @@
       <c r="G7" s="35"/>
     </row>
     <row r="8" spans="1:11">
-      <c r="A8" s="93" t="s">
+      <c r="A8" s="105" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="94"/>
+      <c r="B8" s="106"/>
       <c r="C8" s="10" t="s">
         <v>20</v>
       </c>
@@ -1905,10 +1953,10 @@
       <c r="G8" s="35"/>
     </row>
     <row r="9" spans="1:11">
-      <c r="A9" s="93" t="s">
+      <c r="A9" s="105" t="s">
         <v>26</v>
       </c>
-      <c r="B9" s="94"/>
+      <c r="B9" s="106"/>
       <c r="C9" s="82" t="s">
         <v>30</v>
       </c>
@@ -1924,11 +1972,11 @@
         <v>1</v>
       </c>
       <c r="B10" s="6"/>
-      <c r="C10" s="95" t="s">
+      <c r="C10" s="107" t="s">
         <v>54</v>
       </c>
-      <c r="D10" s="96"/>
-      <c r="E10" s="97"/>
+      <c r="D10" s="108"/>
+      <c r="E10" s="109"/>
       <c r="F10" s="65"/>
       <c r="G10" s="34"/>
       <c r="H10" s="34"/>
@@ -1963,10 +2011,10 @@
       <c r="G12"/>
     </row>
     <row r="13" spans="1:11" s="32" customFormat="1">
-      <c r="A13" s="98" t="s">
+      <c r="A13" s="110" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="99"/>
+      <c r="B13" s="111"/>
       <c r="C13" s="64" t="s">
         <v>14</v>
       </c>
@@ -2109,41 +2157,41 @@
       <c r="K23" s="15"/>
     </row>
     <row r="24" spans="1:11" ht="13.5" customHeight="1">
-      <c r="A24" s="100" t="s">
+      <c r="A24" s="94" t="s">
         <v>7</v>
       </c>
-      <c r="B24" s="100" t="s">
+      <c r="B24" s="94" t="s">
         <v>3</v>
       </c>
-      <c r="C24" s="92" t="s">
+      <c r="C24" s="100" t="s">
         <v>4</v>
       </c>
-      <c r="D24" s="92" t="s">
+      <c r="D24" s="100" t="s">
         <v>6</v>
       </c>
-      <c r="E24" s="92" t="s">
+      <c r="E24" s="100" t="s">
         <v>5</v>
       </c>
-      <c r="F24" s="101" t="s">
+      <c r="F24" s="98" t="s">
         <v>40</v>
       </c>
-      <c r="G24" s="92" t="s">
+      <c r="G24" s="100" t="s">
         <v>1</v>
       </c>
-      <c r="H24" s="92"/>
+      <c r="H24" s="100"/>
       <c r="I24" s="16"/>
       <c r="J24" s="17"/>
       <c r="K24" s="9"/>
     </row>
     <row r="25" spans="1:11">
-      <c r="A25" s="100"/>
-      <c r="B25" s="100"/>
-      <c r="C25" s="92"/>
-      <c r="D25" s="92"/>
-      <c r="E25" s="92"/>
-      <c r="F25" s="102"/>
-      <c r="G25" s="92"/>
-      <c r="H25" s="92"/>
+      <c r="A25" s="94"/>
+      <c r="B25" s="94"/>
+      <c r="C25" s="100"/>
+      <c r="D25" s="100"/>
+      <c r="E25" s="100"/>
+      <c r="F25" s="99"/>
+      <c r="G25" s="100"/>
+      <c r="H25" s="100"/>
       <c r="I25" s="18"/>
       <c r="J25" s="29"/>
       <c r="K25" s="15"/>
@@ -2393,37 +2441,37 @@
       <c r="K43" s="15"/>
     </row>
     <row r="44" spans="1:11" ht="13.5" customHeight="1">
-      <c r="A44" s="100" t="s">
+      <c r="A44" s="94" t="s">
         <v>7</v>
       </c>
-      <c r="B44" s="100" t="s">
+      <c r="B44" s="94" t="s">
         <v>3</v>
       </c>
-      <c r="C44" s="103" t="s">
+      <c r="C44" s="92" t="s">
         <v>4</v>
       </c>
-      <c r="D44" s="104"/>
-      <c r="E44" s="92" t="s">
+      <c r="D44" s="95"/>
+      <c r="E44" s="100" t="s">
         <v>6</v>
       </c>
-      <c r="F44" s="107"/>
-      <c r="G44" s="92" t="s">
+      <c r="F44" s="103"/>
+      <c r="G44" s="100" t="s">
         <v>1</v>
       </c>
-      <c r="H44" s="92"/>
+      <c r="H44" s="100"/>
       <c r="I44" s="16"/>
       <c r="J44" s="17"/>
       <c r="K44" s="9"/>
     </row>
     <row r="45" spans="1:11">
-      <c r="A45" s="100"/>
-      <c r="B45" s="100"/>
-      <c r="C45" s="105"/>
-      <c r="D45" s="106"/>
-      <c r="E45" s="92"/>
-      <c r="F45" s="108"/>
-      <c r="G45" s="92"/>
-      <c r="H45" s="92"/>
+      <c r="A45" s="94"/>
+      <c r="B45" s="94"/>
+      <c r="C45" s="93"/>
+      <c r="D45" s="96"/>
+      <c r="E45" s="100"/>
+      <c r="F45" s="104"/>
+      <c r="G45" s="100"/>
+      <c r="H45" s="100"/>
       <c r="I45" s="18"/>
       <c r="J45" s="29"/>
       <c r="K45" s="15"/>
@@ -2564,37 +2612,37 @@
       <c r="K56" s="15"/>
     </row>
     <row r="57" spans="1:11" ht="13.5" customHeight="1">
-      <c r="A57" s="100" t="s">
+      <c r="A57" s="94" t="s">
         <v>7</v>
       </c>
-      <c r="B57" s="100" t="s">
+      <c r="B57" s="94" t="s">
         <v>3</v>
       </c>
-      <c r="C57" s="103" t="s">
+      <c r="C57" s="92" t="s">
         <v>4</v>
       </c>
-      <c r="D57" s="104"/>
-      <c r="E57" s="92" t="s">
+      <c r="D57" s="95"/>
+      <c r="E57" s="100" t="s">
         <v>6</v>
       </c>
-      <c r="F57" s="107"/>
-      <c r="G57" s="92" t="s">
+      <c r="F57" s="103"/>
+      <c r="G57" s="100" t="s">
         <v>1</v>
       </c>
-      <c r="H57" s="92"/>
+      <c r="H57" s="100"/>
       <c r="I57" s="16"/>
       <c r="J57" s="17"/>
       <c r="K57" s="9"/>
     </row>
     <row r="58" spans="1:11">
-      <c r="A58" s="100"/>
-      <c r="B58" s="100"/>
-      <c r="C58" s="105"/>
-      <c r="D58" s="106"/>
-      <c r="E58" s="92"/>
-      <c r="F58" s="108"/>
-      <c r="G58" s="92"/>
-      <c r="H58" s="92"/>
+      <c r="A58" s="94"/>
+      <c r="B58" s="94"/>
+      <c r="C58" s="93"/>
+      <c r="D58" s="96"/>
+      <c r="E58" s="100"/>
+      <c r="F58" s="104"/>
+      <c r="G58" s="100"/>
+      <c r="H58" s="100"/>
       <c r="I58" s="18"/>
       <c r="J58" s="29"/>
       <c r="K58" s="15"/>
@@ -2828,39 +2876,41 @@
       <c r="K76" s="15"/>
     </row>
     <row r="77" spans="1:11" ht="13.5" customHeight="1">
-      <c r="A77" s="112" t="s">
+      <c r="A77" s="101" t="s">
         <v>7</v>
       </c>
-      <c r="B77" s="112" t="s">
+      <c r="B77" s="101" t="s">
         <v>3</v>
       </c>
-      <c r="C77" s="103" t="s">
+      <c r="C77" s="92" t="s">
         <v>4</v>
       </c>
-      <c r="D77" s="107"/>
-      <c r="E77" s="101" t="s">
+      <c r="D77" s="103"/>
+      <c r="E77" s="98" t="s">
         <v>6</v>
       </c>
-      <c r="F77" s="101" t="s">
+      <c r="F77" s="98" t="s">
         <v>48</v>
       </c>
-      <c r="G77" s="103" t="s">
+      <c r="G77" s="98" t="s">
+        <v>40</v>
+      </c>
+      <c r="H77" s="92" t="s">
         <v>1</v>
       </c>
-      <c r="H77" s="109"/>
       <c r="I77" s="16"/>
       <c r="J77" s="17"/>
       <c r="K77" s="9"/>
     </row>
     <row r="78" spans="1:11">
-      <c r="A78" s="113"/>
-      <c r="B78" s="113"/>
-      <c r="C78" s="105"/>
-      <c r="D78" s="108"/>
-      <c r="E78" s="102"/>
-      <c r="F78" s="102"/>
-      <c r="G78" s="105"/>
-      <c r="H78" s="110"/>
+      <c r="A78" s="102"/>
+      <c r="B78" s="102"/>
+      <c r="C78" s="93"/>
+      <c r="D78" s="104"/>
+      <c r="E78" s="99"/>
+      <c r="F78" s="99"/>
+      <c r="G78" s="99"/>
+      <c r="H78" s="93"/>
       <c r="I78" s="18"/>
       <c r="J78" s="29"/>
       <c r="K78" s="15"/>
@@ -2878,10 +2928,10 @@
       <c r="D79" s="89"/>
       <c r="E79" s="83"/>
       <c r="F79" s="68"/>
-      <c r="G79" s="20" t="s">
+      <c r="G79" s="20"/>
+      <c r="H79" s="112" t="s">
         <v>59</v>
       </c>
-      <c r="H79" s="21"/>
       <c r="I79" s="21"/>
       <c r="J79" s="28"/>
       <c r="K79" s="15"/>
@@ -2901,7 +2951,7 @@
       <c r="E80" s="83"/>
       <c r="F80" s="68"/>
       <c r="G80" s="20"/>
-      <c r="H80" s="21"/>
+      <c r="H80" s="113"/>
       <c r="I80" s="21"/>
       <c r="J80" s="28"/>
       <c r="K80" s="15"/>
@@ -2920,8 +2970,10 @@
       <c r="D81" s="89"/>
       <c r="E81" s="89"/>
       <c r="F81" s="68"/>
-      <c r="G81" s="20"/>
-      <c r="H81" s="21"/>
+      <c r="G81" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="H81" s="113"/>
       <c r="I81" s="21"/>
       <c r="J81" s="22"/>
       <c r="K81" s="15"/>
@@ -2937,7 +2989,7 @@
       <c r="E82" s="83"/>
       <c r="F82" s="68"/>
       <c r="G82" s="20"/>
-      <c r="H82" s="21"/>
+      <c r="H82" s="113"/>
       <c r="I82" s="21"/>
       <c r="J82" s="22"/>
       <c r="K82" s="15"/>
@@ -2953,7 +3005,7 @@
       <c r="E83" s="83"/>
       <c r="F83" s="68"/>
       <c r="G83" s="20"/>
-      <c r="H83" s="21"/>
+      <c r="H83" s="113"/>
       <c r="I83" s="21"/>
       <c r="J83" s="22"/>
       <c r="K83" s="15"/>
@@ -2969,7 +3021,7 @@
       <c r="E84" s="84"/>
       <c r="F84" s="74"/>
       <c r="G84" s="73"/>
-      <c r="H84" s="75"/>
+      <c r="H84" s="114"/>
       <c r="I84" s="75"/>
       <c r="J84" s="76"/>
       <c r="K84" s="15"/>
@@ -2982,7 +3034,7 @@
       <c r="E85" s="85"/>
       <c r="F85" s="69"/>
       <c r="G85" s="25"/>
-      <c r="H85" s="26"/>
+      <c r="H85" s="115"/>
       <c r="I85" s="26"/>
       <c r="J85" s="27"/>
       <c r="K85" s="15"/>
@@ -3015,39 +3067,41 @@
       <c r="K89" s="15"/>
     </row>
     <row r="90" spans="1:11" ht="13.5" customHeight="1">
-      <c r="A90" s="100" t="s">
+      <c r="A90" s="94" t="s">
         <v>7</v>
       </c>
-      <c r="B90" s="100" t="s">
+      <c r="B90" s="94" t="s">
         <v>3</v>
       </c>
-      <c r="C90" s="103" t="s">
+      <c r="C90" s="92" t="s">
         <v>4</v>
       </c>
-      <c r="D90" s="104"/>
-      <c r="E90" s="111" t="s">
+      <c r="D90" s="95"/>
+      <c r="E90" s="97" t="s">
         <v>6</v>
       </c>
-      <c r="F90" s="101" t="s">
+      <c r="F90" s="98" t="s">
         <v>48</v>
       </c>
-      <c r="G90" s="92" t="s">
+      <c r="G90" s="98" t="s">
+        <v>40</v>
+      </c>
+      <c r="H90" s="92" t="s">
         <v>1</v>
       </c>
-      <c r="H90" s="92"/>
       <c r="I90" s="16"/>
       <c r="J90" s="17"/>
       <c r="K90" s="9"/>
     </row>
     <row r="91" spans="1:11">
-      <c r="A91" s="100"/>
-      <c r="B91" s="100"/>
-      <c r="C91" s="105"/>
-      <c r="D91" s="106"/>
-      <c r="E91" s="111"/>
-      <c r="F91" s="102"/>
-      <c r="G91" s="92"/>
-      <c r="H91" s="92"/>
+      <c r="A91" s="94"/>
+      <c r="B91" s="94"/>
+      <c r="C91" s="93"/>
+      <c r="D91" s="96"/>
+      <c r="E91" s="97"/>
+      <c r="F91" s="99"/>
+      <c r="G91" s="99"/>
+      <c r="H91" s="93"/>
       <c r="I91" s="18"/>
       <c r="J91" s="29"/>
       <c r="K91" s="15"/>
@@ -3062,7 +3116,7 @@
       <c r="E92" s="83"/>
       <c r="F92" s="68"/>
       <c r="G92" s="20"/>
-      <c r="H92" s="21"/>
+      <c r="H92" s="112"/>
       <c r="I92" s="21"/>
       <c r="J92" s="28"/>
       <c r="K92" s="15"/>
@@ -3078,7 +3132,7 @@
       <c r="E93" s="83"/>
       <c r="F93" s="68"/>
       <c r="G93" s="20"/>
-      <c r="H93" s="21"/>
+      <c r="H93" s="113"/>
       <c r="I93" s="21"/>
       <c r="J93" s="28"/>
       <c r="K93" s="15"/>
@@ -3094,7 +3148,7 @@
       <c r="E94" s="89"/>
       <c r="F94" s="68"/>
       <c r="G94" s="20"/>
-      <c r="H94" s="21"/>
+      <c r="H94" s="113"/>
       <c r="I94" s="21"/>
       <c r="J94" s="22"/>
       <c r="K94" s="15"/>
@@ -3110,7 +3164,7 @@
       <c r="E95" s="83"/>
       <c r="F95" s="68"/>
       <c r="G95" s="20"/>
-      <c r="H95" s="21"/>
+      <c r="H95" s="113"/>
       <c r="I95" s="21"/>
       <c r="J95" s="22"/>
       <c r="K95" s="15"/>
@@ -3126,7 +3180,7 @@
       <c r="E96" s="83"/>
       <c r="F96" s="68"/>
       <c r="G96" s="20"/>
-      <c r="H96" s="21"/>
+      <c r="H96" s="113"/>
       <c r="I96" s="21"/>
       <c r="J96" s="22"/>
       <c r="K96" s="15"/>
@@ -3142,7 +3196,7 @@
       <c r="E97" s="84"/>
       <c r="F97" s="74"/>
       <c r="G97" s="73"/>
-      <c r="H97" s="75"/>
+      <c r="H97" s="114"/>
       <c r="I97" s="75"/>
       <c r="J97" s="76"/>
       <c r="K97" s="15"/>
@@ -3155,32 +3209,13 @@
       <c r="E98" s="85"/>
       <c r="F98" s="69"/>
       <c r="G98" s="25"/>
-      <c r="H98" s="26"/>
+      <c r="H98" s="115"/>
       <c r="I98" s="26"/>
       <c r="J98" s="27"/>
       <c r="K98" s="15"/>
     </row>
   </sheetData>
-  <mergeCells count="35">
-    <mergeCell ref="G77:H78"/>
-    <mergeCell ref="A90:A91"/>
-    <mergeCell ref="B90:B91"/>
-    <mergeCell ref="C90:D91"/>
-    <mergeCell ref="E90:E91"/>
-    <mergeCell ref="F90:F91"/>
-    <mergeCell ref="G90:H91"/>
-    <mergeCell ref="A77:A78"/>
-    <mergeCell ref="B77:B78"/>
-    <mergeCell ref="C77:D78"/>
-    <mergeCell ref="E77:E78"/>
-    <mergeCell ref="F77:F78"/>
-    <mergeCell ref="C44:D45"/>
-    <mergeCell ref="F44:F45"/>
-    <mergeCell ref="A57:A58"/>
-    <mergeCell ref="B57:B58"/>
-    <mergeCell ref="C57:D58"/>
-    <mergeCell ref="E57:E58"/>
-    <mergeCell ref="F57:F58"/>
+  <mergeCells count="37">
     <mergeCell ref="G44:H45"/>
     <mergeCell ref="G57:H58"/>
     <mergeCell ref="A9:B9"/>
@@ -3197,6 +3232,27 @@
     <mergeCell ref="A44:A45"/>
     <mergeCell ref="B44:B45"/>
     <mergeCell ref="E44:E45"/>
+    <mergeCell ref="C44:D45"/>
+    <mergeCell ref="F44:F45"/>
+    <mergeCell ref="A57:A58"/>
+    <mergeCell ref="B57:B58"/>
+    <mergeCell ref="C57:D58"/>
+    <mergeCell ref="E57:E58"/>
+    <mergeCell ref="F57:F58"/>
+    <mergeCell ref="A90:A91"/>
+    <mergeCell ref="B90:B91"/>
+    <mergeCell ref="C90:D91"/>
+    <mergeCell ref="E90:E91"/>
+    <mergeCell ref="F90:F91"/>
+    <mergeCell ref="A77:A78"/>
+    <mergeCell ref="B77:B78"/>
+    <mergeCell ref="C77:D78"/>
+    <mergeCell ref="E77:E78"/>
+    <mergeCell ref="F77:F78"/>
+    <mergeCell ref="G77:G78"/>
+    <mergeCell ref="H77:H78"/>
+    <mergeCell ref="G90:G91"/>
+    <mergeCell ref="H90:H91"/>
   </mergeCells>
   <phoneticPr fontId="3"/>
   <dataValidations count="3">
@@ -3206,7 +3262,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C12" xr:uid="{CCFC1331-CEEF-574E-9BCC-37D38F486896}">
       <formula1>adjustFieldName</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F26:F32 F92:F98 F79:F85" xr:uid="{18C70D90-9F1A-D84D-9F1C-490DE84E2C64}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F26:F32 F92:G98 F79:G85" xr:uid="{18C70D90-9F1A-D84D-9F1C-490DE84E2C64}">
       <formula1>yesNo</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>